<commit_message>
Update BOM-speeduino compatible PCB for m52 rev2.0 sequential.xlsx
</commit_message>
<xml_diff>
--- a/m52 PnP/Rev2.0 documents/BOM-speeduino compatible PCB for m52 rev2.0 sequential.xlsx
+++ b/m52 PnP/Rev2.0 documents/BOM-speeduino compatible PCB for m52 rev2.0 sequential.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\Rev2.0 documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADA64B4B-E22B-449F-A9DC-E0D48585DE33}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BC6CE9-E78C-49C5-95DF-8F309DA2720D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3225" yWindow="2640" windowWidth="23475" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="31425" yWindow="2100" windowWidth="23475" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="361" uniqueCount="297">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="294">
   <si>
     <t>Value</t>
   </si>
@@ -899,9 +899,6 @@
     <t>WM3702-ND</t>
   </si>
   <si>
-    <t>Hardware for motronic case</t>
-  </si>
-  <si>
     <r>
       <t>C19,</t>
     </r>
@@ -913,15 +910,6 @@
       </rPr>
       <t>C27</t>
     </r>
-  </si>
-  <si>
-    <t>Speeduino vr-conditioner</t>
-  </si>
-  <si>
-    <t>vr-conditioner</t>
-  </si>
-  <si>
-    <t>max 9926 vr-conditioner</t>
   </si>
   <si>
     <r>
@@ -1241,6 +1229,9 @@
   </si>
   <si>
     <t>Q1,Q2,Q3,Q4,Q5,Q6</t>
+  </si>
+  <si>
+    <t>Hardware for ms41 case</t>
   </si>
 </sst>
 </file>
@@ -2018,10 +2009,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S64"/>
+  <dimension ref="A1:S63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A25" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+    <sheetView tabSelected="1" topLeftCell="A41" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="B49" sqref="B49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -2436,7 +2427,7 @@
         <v>2</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C8" s="3" t="s">
         <v>16</v>
@@ -2498,7 +2489,7 @@
         <v>5</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>294</v>
+        <v>290</v>
       </c>
       <c r="C9" s="3" t="s">
         <v>17</v>
@@ -2560,13 +2551,13 @@
         <v>1</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>270</v>
+        <v>266</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>271</v>
+        <v>267</v>
       </c>
       <c r="D10" s="3" t="s">
-        <v>273</v>
+        <v>269</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>11</v>
@@ -2576,13 +2567,13 @@
         <v>9</v>
       </c>
       <c r="H10" s="3" t="s">
-        <v>272</v>
+        <v>268</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>275</v>
+        <v>271</v>
       </c>
       <c r="J10" s="33" t="s">
-        <v>274</v>
+        <v>270</v>
       </c>
       <c r="K10" s="5">
         <v>0.3</v>
@@ -2713,7 +2704,7 @@
         <v>2</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>247</v>
+        <v>243</v>
       </c>
       <c r="C13" s="3" t="s">
         <v>92</v>
@@ -2775,7 +2766,7 @@
         <v>3</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>250</v>
+        <v>246</v>
       </c>
       <c r="C14" s="3" t="s">
         <v>93</v>
@@ -2837,7 +2828,7 @@
         <v>12</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>278</v>
+        <v>274</v>
       </c>
       <c r="C15" s="3" t="s">
         <v>27</v>
@@ -2897,7 +2888,7 @@
         <v>8</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>282</v>
+        <v>278</v>
       </c>
       <c r="C16" s="3" t="s">
         <v>28</v>
@@ -3416,7 +3407,7 @@
         <v>6</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>296</v>
+        <v>292</v>
       </c>
       <c r="C26" s="3" t="s">
         <v>89</v>
@@ -3541,13 +3532,13 @@
         <v>1</v>
       </c>
       <c r="B28" s="28" t="s">
-        <v>251</v>
+        <v>247</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>252</v>
+        <v>248</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>253</v>
+        <v>249</v>
       </c>
       <c r="E28" s="3" t="s">
         <v>195</v>
@@ -3557,13 +3548,13 @@
         <v>20</v>
       </c>
       <c r="H28" s="3" t="s">
-        <v>254</v>
+        <v>250</v>
       </c>
       <c r="I28" s="26" t="s">
-        <v>256</v>
+        <v>252</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>255</v>
+        <v>251</v>
       </c>
       <c r="K28" s="6">
         <v>0.25</v>
@@ -3751,7 +3742,7 @@
         <v>22</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>295</v>
+        <v>291</v>
       </c>
       <c r="C32" s="3" t="s">
         <v>43</v>
@@ -3811,7 +3802,7 @@
         <v>6</v>
       </c>
       <c r="B33" s="11" t="s">
-        <v>281</v>
+        <v>277</v>
       </c>
       <c r="C33" s="12">
         <v>680</v>
@@ -3933,7 +3924,7 @@
         <v>9</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>279</v>
+        <v>275</v>
       </c>
       <c r="C35" s="3" t="s">
         <v>164</v>
@@ -3995,7 +3986,7 @@
         <v>3</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>248</v>
+        <v>244</v>
       </c>
       <c r="C36" s="3" t="s">
         <v>91</v>
@@ -4057,7 +4048,7 @@
         <v>16</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>277</v>
+        <v>273</v>
       </c>
       <c r="C37" s="3" t="s">
         <v>54</v>
@@ -4117,27 +4108,27 @@
         <v>6</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>280</v>
+        <v>276</v>
       </c>
       <c r="C38" s="3">
         <v>150</v>
       </c>
       <c r="D38" s="3" t="s">
-        <v>288</v>
+        <v>284</v>
       </c>
       <c r="E38" s="3"/>
       <c r="F38" s="3"/>
       <c r="G38" s="3" t="s">
-        <v>289</v>
+        <v>285</v>
       </c>
       <c r="H38" s="3" t="s">
-        <v>291</v>
+        <v>287</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>292</v>
+        <v>288</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>290</v>
+        <v>286</v>
       </c>
       <c r="K38" s="5">
         <v>0.27</v>
@@ -4177,7 +4168,7 @@
         <v>2</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>249</v>
+        <v>245</v>
       </c>
       <c r="C39" s="3" t="s">
         <v>180</v>
@@ -4194,7 +4185,7 @@
         <v>182</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>293</v>
+        <v>289</v>
       </c>
       <c r="J39" s="2" t="s">
         <v>183</v>
@@ -4327,29 +4318,29 @@
         <v>1</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>257</v>
+        <v>253</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>258</v>
+        <v>254</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>259</v>
+        <v>255</v>
       </c>
       <c r="E42" s="3" t="s">
-        <v>260</v>
+        <v>256</v>
       </c>
       <c r="F42" s="3"/>
       <c r="G42" s="3" t="s">
         <v>38</v>
       </c>
       <c r="H42" s="3" t="s">
+        <v>254</v>
+      </c>
+      <c r="I42" s="30" t="s">
+        <v>257</v>
+      </c>
+      <c r="J42" s="2" t="s">
         <v>258</v>
-      </c>
-      <c r="I42" s="30" t="s">
-        <v>261</v>
-      </c>
-      <c r="J42" s="2" t="s">
-        <v>262</v>
       </c>
       <c r="K42" s="5">
         <v>0.59</v>
@@ -4365,16 +4356,16 @@
       </c>
       <c r="O42" s="4"/>
       <c r="P42" s="4" t="s">
-        <v>263</v>
+        <v>259</v>
       </c>
       <c r="Q42" t="s">
-        <v>264</v>
+        <v>260</v>
       </c>
       <c r="R42" t="s">
-        <v>265</v>
+        <v>261</v>
       </c>
       <c r="S42" t="s">
-        <v>266</v>
+        <v>262</v>
       </c>
     </row>
     <row r="43" spans="1:19" ht="26.25" thickBot="1">
@@ -4507,7 +4498,7 @@
         <v>3</v>
       </c>
       <c r="B45" s="11" t="s">
-        <v>276</v>
+        <v>272</v>
       </c>
       <c r="C45" s="12" t="s">
         <v>94</v>
@@ -4631,13 +4622,13 @@
         <v>2</v>
       </c>
       <c r="B47" s="11" t="s">
-        <v>287</v>
+        <v>283</v>
       </c>
       <c r="C47" s="12" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="D47" s="3" t="s">
-        <v>283</v>
+        <v>279</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>217</v>
@@ -4647,13 +4638,13 @@
         <v>38</v>
       </c>
       <c r="H47" s="12" t="s">
-        <v>284</v>
+        <v>280</v>
       </c>
       <c r="I47" s="12" t="s">
-        <v>285</v>
+        <v>281</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>286</v>
+        <v>282</v>
       </c>
       <c r="K47" s="6">
         <v>1.41</v>
@@ -4715,7 +4706,7 @@
     <row r="49" spans="1:19" ht="16.5" thickBot="1">
       <c r="A49" s="15"/>
       <c r="B49" s="4" t="s">
-        <v>241</v>
+        <v>293</v>
       </c>
       <c r="C49" s="3"/>
       <c r="D49" s="3"/>
@@ -4739,46 +4730,77 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="25.5" customHeight="1" thickBot="1">
+    <row r="50" spans="1:19" ht="16.5" thickBot="1">
       <c r="A50" s="17">
         <v>1</v>
       </c>
       <c r="B50" s="11" t="s">
-        <v>244</v>
+        <v>229</v>
       </c>
       <c r="C50" s="12" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="D50" s="3" t="s">
-        <v>243</v>
-      </c>
-      <c r="E50" s="3" t="s">
-        <v>96</v>
-      </c>
+        <v>236</v>
+      </c>
+      <c r="E50" s="3"/>
       <c r="F50" s="12"/>
-      <c r="G50" s="12"/>
-      <c r="H50" s="12"/>
-      <c r="I50" s="12"/>
-      <c r="J50" s="2"/>
-      <c r="K50" s="6"/>
-      <c r="L50" s="6"/>
-      <c r="M50" s="6"/>
-      <c r="N50" s="6"/>
+      <c r="G50" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K50" s="6">
+        <v>0.33</v>
+      </c>
+      <c r="L50" s="6">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="M50" s="6">
+        <f>K50*A50</f>
+        <v>0.33</v>
+      </c>
+      <c r="N50" s="6">
+        <f>L50*A50</f>
+        <v>0.38200000000000001</v>
+      </c>
       <c r="O50" s="4"/>
-      <c r="P50" s="4"/>
+      <c r="P50" s="4" t="str">
+        <f>IF(NOT(I50=""),A50&amp;","&amp;I50,"")</f>
+        <v>1,WM3702-ND</v>
+      </c>
+      <c r="Q50" t="str">
+        <f>A50&amp;"x "&amp;C50</f>
+        <v>1x 6-POS connector</v>
+      </c>
+      <c r="R50" t="str">
+        <f>IF(NOT(J50=""),J50&amp;"|"&amp;A50,"")</f>
+        <v>538-39-01-2060|1</v>
+      </c>
+      <c r="S50" t="str">
+        <f>H50&amp;" "&amp;A50</f>
+        <v>39-01-2060 1</v>
+      </c>
     </row>
     <row r="51" spans="1:19" ht="16.5" thickBot="1">
       <c r="A51" s="17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="12"/>
@@ -4786,108 +4808,69 @@
         <v>192</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="K51" s="6">
-        <v>0.33</v>
+        <v>0.16</v>
       </c>
       <c r="L51" s="6">
-        <v>0.38200000000000001</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="M51" s="6">
         <f>K51*A51</f>
-        <v>0.33</v>
+        <v>0.96</v>
       </c>
       <c r="N51" s="6">
         <f>L51*A51</f>
-        <v>0.38200000000000001</v>
+        <v>1.0859999999999999</v>
       </c>
       <c r="O51" s="4"/>
       <c r="P51" s="4" t="str">
         <f>IF(NOT(I51=""),A51&amp;","&amp;I51,"")</f>
-        <v>1,WM3702-ND</v>
+        <v>6,WM9154-ND</v>
       </c>
       <c r="Q51" t="str">
         <f>A51&amp;"x "&amp;C51</f>
-        <v>1x 6-POS connector</v>
+        <v>6x Female pin</v>
       </c>
       <c r="R51" t="str">
         <f>IF(NOT(J51=""),J51&amp;"|"&amp;A51,"")</f>
-        <v>538-39-01-2060|1</v>
+        <v>538-39-00-0078|6</v>
       </c>
       <c r="S51" t="str">
         <f>H51&amp;" "&amp;A51</f>
-        <v>39-01-2060 1</v>
+        <v>39-00-0078 6</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A52" s="17">
-        <v>6</v>
-      </c>
-      <c r="B52" s="11" t="s">
-        <v>230</v>
-      </c>
-      <c r="C52" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="D52" s="3" t="s">
-        <v>232</v>
-      </c>
+      <c r="A52" s="15"/>
+      <c r="B52" s="11"/>
+      <c r="C52" s="12"/>
+      <c r="D52" s="3"/>
       <c r="E52" s="3"/>
       <c r="F52" s="12"/>
-      <c r="G52" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="H52" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="I52" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="J52" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="K52" s="6">
-        <v>0.16</v>
-      </c>
-      <c r="L52" s="6">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="M52" s="6">
-        <f>K52*A52</f>
-        <v>0.96</v>
-      </c>
-      <c r="N52" s="6">
-        <f>L52*A52</f>
-        <v>1.0859999999999999</v>
-      </c>
+      <c r="G52" s="12"/>
+      <c r="H52" s="12"/>
+      <c r="I52" s="12"/>
+      <c r="J52" s="2"/>
+      <c r="K52" s="6"/>
+      <c r="L52" s="6"/>
+      <c r="M52" s="6"/>
+      <c r="N52" s="6"/>
       <c r="O52" s="4"/>
-      <c r="P52" s="4" t="str">
-        <f>IF(NOT(I52=""),A52&amp;","&amp;I52,"")</f>
-        <v>6,WM9154-ND</v>
-      </c>
-      <c r="Q52" t="str">
-        <f>A52&amp;"x "&amp;C52</f>
-        <v>6x Female pin</v>
-      </c>
-      <c r="R52" t="str">
-        <f>IF(NOT(J52=""),J52&amp;"|"&amp;A52,"")</f>
-        <v>538-39-00-0078|6</v>
-      </c>
-      <c r="S52" t="str">
-        <f>H52&amp;" "&amp;A52</f>
-        <v>39-00-0078 6</v>
-      </c>
+      <c r="P52" s="4"/>
     </row>
     <row r="53" spans="1:19" ht="16.5" thickBot="1">
       <c r="A53" s="15"/>
-      <c r="B53" s="11"/>
+      <c r="B53" s="11" t="s">
+        <v>263</v>
+      </c>
       <c r="C53" s="12"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -4904,37 +4887,76 @@
       <c r="P53" s="4"/>
     </row>
     <row r="54" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A54" s="15"/>
-      <c r="B54" s="11" t="s">
-        <v>267</v>
-      </c>
-      <c r="C54" s="12"/>
-      <c r="D54" s="3"/>
+      <c r="A54" s="17">
+        <v>1</v>
+      </c>
+      <c r="B54" s="32" t="s">
+        <v>229</v>
+      </c>
+      <c r="C54" s="12" t="s">
+        <v>237</v>
+      </c>
+      <c r="D54" s="3" t="s">
+        <v>236</v>
+      </c>
       <c r="E54" s="3"/>
       <c r="F54" s="12"/>
-      <c r="G54" s="12"/>
-      <c r="H54" s="12"/>
-      <c r="I54" s="12"/>
-      <c r="J54" s="2"/>
-      <c r="K54" s="6"/>
-      <c r="L54" s="6"/>
-      <c r="M54" s="6"/>
-      <c r="N54" s="6"/>
+      <c r="G54" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="H54" s="12" t="s">
+        <v>238</v>
+      </c>
+      <c r="I54" s="12" t="s">
+        <v>240</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>239</v>
+      </c>
+      <c r="K54" s="6">
+        <v>0.33</v>
+      </c>
+      <c r="L54" s="6">
+        <v>0.38200000000000001</v>
+      </c>
+      <c r="M54" s="6">
+        <f>K54*A54</f>
+        <v>0.33</v>
+      </c>
+      <c r="N54" s="6">
+        <f>L54*A54</f>
+        <v>0.38200000000000001</v>
+      </c>
       <c r="O54" s="4"/>
-      <c r="P54" s="4"/>
+      <c r="P54" s="4" t="str">
+        <f>IF(NOT(I54=""),A54&amp;","&amp;I54,"")</f>
+        <v>1,WM3702-ND</v>
+      </c>
+      <c r="Q54" t="str">
+        <f>A54&amp;"x "&amp;C54</f>
+        <v>1x 6-POS connector</v>
+      </c>
+      <c r="R54" t="str">
+        <f>IF(NOT(J54=""),J54&amp;"|"&amp;A54,"")</f>
+        <v>538-39-01-2060|1</v>
+      </c>
+      <c r="S54" t="str">
+        <f>H54&amp;" "&amp;A54</f>
+        <v>39-01-2060 1</v>
+      </c>
     </row>
     <row r="55" spans="1:19" ht="16.5" thickBot="1">
       <c r="A55" s="17">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>229</v>
+        <v>230</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>236</v>
+        <v>232</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="12"/>
@@ -4942,157 +4964,98 @@
         <v>192</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>239</v>
+        <v>235</v>
       </c>
       <c r="K55" s="6">
-        <v>0.33</v>
+        <v>0.16</v>
       </c>
       <c r="L55" s="6">
-        <v>0.38200000000000001</v>
+        <v>0.18099999999999999</v>
       </c>
       <c r="M55" s="6">
         <f>K55*A55</f>
-        <v>0.33</v>
+        <v>0.96</v>
       </c>
       <c r="N55" s="6">
         <f>L55*A55</f>
-        <v>0.38200000000000001</v>
+        <v>1.0859999999999999</v>
       </c>
       <c r="O55" s="4"/>
       <c r="P55" s="4" t="str">
         <f>IF(NOT(I55=""),A55&amp;","&amp;I55,"")</f>
-        <v>1,WM3702-ND</v>
+        <v>6,WM9154-ND</v>
       </c>
       <c r="Q55" t="str">
         <f>A55&amp;"x "&amp;C55</f>
-        <v>1x 6-POS connector</v>
+        <v>6x Female pin</v>
       </c>
       <c r="R55" t="str">
         <f>IF(NOT(J55=""),J55&amp;"|"&amp;A55,"")</f>
-        <v>538-39-01-2060|1</v>
+        <v>538-39-00-0078|6</v>
       </c>
       <c r="S55" t="str">
         <f>H55&amp;" "&amp;A55</f>
-        <v>39-01-2060 1</v>
-      </c>
-    </row>
-    <row r="56" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A56" s="17">
-        <v>6</v>
-      </c>
-      <c r="B56" s="32" t="s">
-        <v>230</v>
-      </c>
-      <c r="C56" s="12" t="s">
-        <v>231</v>
-      </c>
-      <c r="D56" s="3" t="s">
-        <v>232</v>
-      </c>
+        <v>39-00-0078 6</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" ht="24" customHeight="1" thickBot="1">
+      <c r="A56" s="15"/>
+      <c r="B56" s="4"/>
+      <c r="C56" s="3"/>
+      <c r="D56" s="3"/>
       <c r="E56" s="3"/>
-      <c r="F56" s="12"/>
-      <c r="G56" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="H56" s="12" t="s">
-        <v>233</v>
-      </c>
-      <c r="I56" s="12" t="s">
-        <v>234</v>
-      </c>
-      <c r="J56" s="2" t="s">
-        <v>235</v>
-      </c>
-      <c r="K56" s="6">
-        <v>0.16</v>
-      </c>
-      <c r="L56" s="6">
-        <v>0.18099999999999999</v>
-      </c>
-      <c r="M56" s="6">
-        <f>K56*A56</f>
-        <v>0.96</v>
-      </c>
-      <c r="N56" s="6">
-        <f>L56*A56</f>
-        <v>1.0859999999999999</v>
-      </c>
-      <c r="O56" s="4"/>
-      <c r="P56" s="4" t="str">
-        <f>IF(NOT(I56=""),A56&amp;","&amp;I56,"")</f>
-        <v>6,WM9154-ND</v>
-      </c>
-      <c r="Q56" t="str">
-        <f>A56&amp;"x "&amp;C56</f>
-        <v>6x Female pin</v>
-      </c>
-      <c r="R56" t="str">
-        <f>IF(NOT(J56=""),J56&amp;"|"&amp;A56,"")</f>
-        <v>538-39-00-0078|6</v>
-      </c>
-      <c r="S56" t="str">
-        <f>H56&amp;" "&amp;A56</f>
-        <v>39-00-0078 6</v>
-      </c>
-    </row>
-    <row r="57" spans="1:19" ht="24" customHeight="1" thickBot="1">
-      <c r="A57" s="15"/>
-      <c r="B57" s="4"/>
-      <c r="C57" s="3"/>
-      <c r="D57" s="3"/>
-      <c r="E57" s="3"/>
-      <c r="F57" s="20"/>
-      <c r="G57" s="4"/>
-      <c r="H57" s="34" t="s">
+      <c r="F56" s="20"/>
+      <c r="G56" s="4"/>
+      <c r="H56" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="I57" s="35"/>
-      <c r="J57" s="29"/>
-      <c r="K57" s="1" t="s">
+      <c r="I56" s="35"/>
+      <c r="J56" s="29"/>
+      <c r="K56" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L57" s="1"/>
-      <c r="M57" s="10">
-        <f>SUM(M3:M52)</f>
+      <c r="L56" s="1"/>
+      <c r="M56" s="10">
+        <f>SUM(M3:M51)</f>
         <v>108.58</v>
       </c>
-      <c r="N57" s="10">
-        <f>SUM(N3:N52)</f>
+      <c r="N56" s="10">
+        <f>SUM(N3:N51)</f>
         <v>125.822</v>
       </c>
-      <c r="O57" s="9" t="s">
+      <c r="O56" s="9" t="s">
         <v>65</v>
+      </c>
+    </row>
+    <row r="60" spans="1:19">
+      <c r="B60" t="s">
+        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:19">
       <c r="B61" t="s">
-        <v>219</v>
+        <v>265</v>
       </c>
     </row>
     <row r="62" spans="1:19">
       <c r="B62" t="s">
-        <v>269</v>
+        <v>242</v>
       </c>
     </row>
     <row r="63" spans="1:19">
       <c r="B63" t="s">
-        <v>246</v>
-      </c>
-    </row>
-    <row r="64" spans="1:19">
-      <c r="B64" t="s">
-        <v>268</v>
+        <v>264</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H57:I57"/>
+    <mergeCell ref="H56:I56"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>
@@ -5109,7 +5072,7 @@
     <hyperlink ref="I37" r:id="rId11" xr:uid="{00000000-0004-0000-0000-00000A000000}"/>
   </hyperlinks>
   <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" scale="31" orientation="landscape" horizontalDpi="4294967292" verticalDpi="4294967292" r:id="rId12"/>
+  <pageSetup paperSize="9" scale="21" orientation="portrait" r:id="rId12"/>
   <legacyDrawing r:id="rId13"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fixes to BOM files
</commit_message>
<xml_diff>
--- a/m52 PnP/Rev2.0 documents/BOM-speeduino compatible PCB for m52 rev2.0 sequential.xlsx
+++ b/m52 PnP/Rev2.0 documents/BOM-speeduino compatible PCB for m52 rev2.0 sequential.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\Rev2.0 documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06BC6CE9-E78C-49C5-95DF-8F309DA2720D}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6536DA53-C00E-4732-B81C-BD1D094FE030}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31425" yWindow="2100" windowWidth="23475" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="16785" yWindow="2190" windowWidth="23475" windowHeight="12540" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="294">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="358" uniqueCount="294">
   <si>
     <t>Value</t>
   </si>
@@ -2009,10 +2009,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:S63"/>
+  <dimension ref="A1:S64"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A41" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="B49" sqref="B49"/>
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4731,76 +4731,44 @@
       </c>
     </row>
     <row r="50" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A50" s="17">
-        <v>1</v>
-      </c>
-      <c r="B50" s="11" t="s">
-        <v>229</v>
-      </c>
-      <c r="C50" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="D50" s="3" t="s">
-        <v>236</v>
-      </c>
+      <c r="A50" s="15"/>
+      <c r="B50" s="4" t="s">
+        <v>293</v>
+      </c>
+      <c r="C50" s="3"/>
+      <c r="D50" s="3"/>
       <c r="E50" s="3"/>
-      <c r="F50" s="12"/>
-      <c r="G50" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="H50" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="I50" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="J50" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="K50" s="6">
-        <v>0.33</v>
-      </c>
-      <c r="L50" s="6">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="M50" s="6">
-        <f>K50*A50</f>
-        <v>0.33</v>
-      </c>
-      <c r="N50" s="6">
-        <f>L50*A50</f>
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="O50" s="4"/>
+      <c r="F50" s="3"/>
+      <c r="G50" s="4"/>
+      <c r="H50" s="8"/>
+      <c r="I50" s="3"/>
+      <c r="J50" s="3"/>
+      <c r="K50" s="1"/>
+      <c r="L50" s="1"/>
+      <c r="M50" s="9"/>
+      <c r="N50" s="6"/>
+      <c r="O50" s="9"/>
       <c r="P50" s="4" t="str">
-        <f>IF(NOT(I50=""),A50&amp;","&amp;I50,"")</f>
-        <v>1,WM3702-ND</v>
-      </c>
-      <c r="Q50" t="str">
-        <f>A50&amp;"x "&amp;C50</f>
-        <v>1x 6-POS connector</v>
+        <f t="shared" ref="P50" si="19">IF(NOT(I50=""),A50&amp;","&amp;I50,"")</f>
+        <v/>
       </c>
       <c r="R50" t="str">
-        <f>IF(NOT(J50=""),J50&amp;"|"&amp;A50,"")</f>
-        <v>538-39-01-2060|1</v>
-      </c>
-      <c r="S50" t="str">
-        <f>H50&amp;" "&amp;A50</f>
-        <v>39-01-2060 1</v>
+        <f t="shared" ref="R50" si="20">IF(NOT(J50=""),J50&amp;"|"&amp;A50,"")</f>
+        <v/>
       </c>
     </row>
     <row r="51" spans="1:19" ht="16.5" thickBot="1">
       <c r="A51" s="17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B51" s="11" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C51" s="12" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="D51" s="3" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E51" s="3"/>
       <c r="F51" s="12"/>
@@ -4808,69 +4776,108 @@
         <v>192</v>
       </c>
       <c r="H51" s="12" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="I51" s="12" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="J51" s="2" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="K51" s="6">
-        <v>0.16</v>
+        <v>0.33</v>
       </c>
       <c r="L51" s="6">
-        <v>0.18099999999999999</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="M51" s="6">
         <f>K51*A51</f>
-        <v>0.96</v>
+        <v>0.33</v>
       </c>
       <c r="N51" s="6">
         <f>L51*A51</f>
-        <v>1.0859999999999999</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="O51" s="4"/>
       <c r="P51" s="4" t="str">
         <f>IF(NOT(I51=""),A51&amp;","&amp;I51,"")</f>
-        <v>6,WM9154-ND</v>
+        <v>1,WM3702-ND</v>
       </c>
       <c r="Q51" t="str">
         <f>A51&amp;"x "&amp;C51</f>
-        <v>6x Female pin</v>
+        <v>1x 6-POS connector</v>
       </c>
       <c r="R51" t="str">
         <f>IF(NOT(J51=""),J51&amp;"|"&amp;A51,"")</f>
-        <v>538-39-00-0078|6</v>
+        <v>538-39-01-2060|1</v>
       </c>
       <c r="S51" t="str">
         <f>H51&amp;" "&amp;A51</f>
-        <v>39-00-0078 6</v>
+        <v>39-01-2060 1</v>
       </c>
     </row>
     <row r="52" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A52" s="15"/>
-      <c r="B52" s="11"/>
-      <c r="C52" s="12"/>
-      <c r="D52" s="3"/>
+      <c r="A52" s="17">
+        <v>6</v>
+      </c>
+      <c r="B52" s="11" t="s">
+        <v>230</v>
+      </c>
+      <c r="C52" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="D52" s="3" t="s">
+        <v>232</v>
+      </c>
       <c r="E52" s="3"/>
       <c r="F52" s="12"/>
-      <c r="G52" s="12"/>
-      <c r="H52" s="12"/>
-      <c r="I52" s="12"/>
-      <c r="J52" s="2"/>
-      <c r="K52" s="6"/>
-      <c r="L52" s="6"/>
-      <c r="M52" s="6"/>
-      <c r="N52" s="6"/>
+      <c r="G52" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="H52" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="I52" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="J52" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="K52" s="6">
+        <v>0.16</v>
+      </c>
+      <c r="L52" s="6">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="M52" s="6">
+        <f>K52*A52</f>
+        <v>0.96</v>
+      </c>
+      <c r="N52" s="6">
+        <f>L52*A52</f>
+        <v>1.0859999999999999</v>
+      </c>
       <c r="O52" s="4"/>
-      <c r="P52" s="4"/>
+      <c r="P52" s="4" t="str">
+        <f>IF(NOT(I52=""),A52&amp;","&amp;I52,"")</f>
+        <v>6,WM9154-ND</v>
+      </c>
+      <c r="Q52" t="str">
+        <f>A52&amp;"x "&amp;C52</f>
+        <v>6x Female pin</v>
+      </c>
+      <c r="R52" t="str">
+        <f>IF(NOT(J52=""),J52&amp;"|"&amp;A52,"")</f>
+        <v>538-39-00-0078|6</v>
+      </c>
+      <c r="S52" t="str">
+        <f>H52&amp;" "&amp;A52</f>
+        <v>39-00-0078 6</v>
+      </c>
     </row>
     <row r="53" spans="1:19" ht="16.5" thickBot="1">
       <c r="A53" s="15"/>
-      <c r="B53" s="11" t="s">
-        <v>263</v>
-      </c>
+      <c r="B53" s="11"/>
       <c r="C53" s="12"/>
       <c r="D53" s="3"/>
       <c r="E53" s="3"/>
@@ -4887,76 +4894,37 @@
       <c r="P53" s="4"/>
     </row>
     <row r="54" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A54" s="17">
-        <v>1</v>
-      </c>
-      <c r="B54" s="32" t="s">
-        <v>229</v>
-      </c>
-      <c r="C54" s="12" t="s">
-        <v>237</v>
-      </c>
-      <c r="D54" s="3" t="s">
-        <v>236</v>
-      </c>
+      <c r="A54" s="15"/>
+      <c r="B54" s="11" t="s">
+        <v>263</v>
+      </c>
+      <c r="C54" s="12"/>
+      <c r="D54" s="3"/>
       <c r="E54" s="3"/>
       <c r="F54" s="12"/>
-      <c r="G54" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="H54" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="I54" s="12" t="s">
-        <v>240</v>
-      </c>
-      <c r="J54" s="2" t="s">
-        <v>239</v>
-      </c>
-      <c r="K54" s="6">
-        <v>0.33</v>
-      </c>
-      <c r="L54" s="6">
-        <v>0.38200000000000001</v>
-      </c>
-      <c r="M54" s="6">
-        <f>K54*A54</f>
-        <v>0.33</v>
-      </c>
-      <c r="N54" s="6">
-        <f>L54*A54</f>
-        <v>0.38200000000000001</v>
-      </c>
+      <c r="G54" s="12"/>
+      <c r="H54" s="12"/>
+      <c r="I54" s="12"/>
+      <c r="J54" s="2"/>
+      <c r="K54" s="6"/>
+      <c r="L54" s="6"/>
+      <c r="M54" s="6"/>
+      <c r="N54" s="6"/>
       <c r="O54" s="4"/>
-      <c r="P54" s="4" t="str">
-        <f>IF(NOT(I54=""),A54&amp;","&amp;I54,"")</f>
-        <v>1,WM3702-ND</v>
-      </c>
-      <c r="Q54" t="str">
-        <f>A54&amp;"x "&amp;C54</f>
-        <v>1x 6-POS connector</v>
-      </c>
-      <c r="R54" t="str">
-        <f>IF(NOT(J54=""),J54&amp;"|"&amp;A54,"")</f>
-        <v>538-39-01-2060|1</v>
-      </c>
-      <c r="S54" t="str">
-        <f>H54&amp;" "&amp;A54</f>
-        <v>39-01-2060 1</v>
-      </c>
+      <c r="P54" s="4"/>
     </row>
     <row r="55" spans="1:19" ht="16.5" thickBot="1">
       <c r="A55" s="17">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="B55" s="32" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C55" s="12" t="s">
-        <v>231</v>
+        <v>237</v>
       </c>
       <c r="D55" s="3" t="s">
-        <v>232</v>
+        <v>236</v>
       </c>
       <c r="E55" s="3"/>
       <c r="F55" s="12"/>
@@ -4964,98 +4932,157 @@
         <v>192</v>
       </c>
       <c r="H55" s="12" t="s">
-        <v>233</v>
+        <v>238</v>
       </c>
       <c r="I55" s="12" t="s">
-        <v>234</v>
+        <v>240</v>
       </c>
       <c r="J55" s="2" t="s">
-        <v>235</v>
+        <v>239</v>
       </c>
       <c r="K55" s="6">
-        <v>0.16</v>
+        <v>0.33</v>
       </c>
       <c r="L55" s="6">
-        <v>0.18099999999999999</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="M55" s="6">
         <f>K55*A55</f>
-        <v>0.96</v>
+        <v>0.33</v>
       </c>
       <c r="N55" s="6">
         <f>L55*A55</f>
-        <v>1.0859999999999999</v>
+        <v>0.38200000000000001</v>
       </c>
       <c r="O55" s="4"/>
       <c r="P55" s="4" t="str">
         <f>IF(NOT(I55=""),A55&amp;","&amp;I55,"")</f>
-        <v>6,WM9154-ND</v>
+        <v>1,WM3702-ND</v>
       </c>
       <c r="Q55" t="str">
         <f>A55&amp;"x "&amp;C55</f>
-        <v>6x Female pin</v>
+        <v>1x 6-POS connector</v>
       </c>
       <c r="R55" t="str">
         <f>IF(NOT(J55=""),J55&amp;"|"&amp;A55,"")</f>
-        <v>538-39-00-0078|6</v>
+        <v>538-39-01-2060|1</v>
       </c>
       <c r="S55" t="str">
         <f>H55&amp;" "&amp;A55</f>
+        <v>39-01-2060 1</v>
+      </c>
+    </row>
+    <row r="56" spans="1:19" ht="16.5" thickBot="1">
+      <c r="A56" s="17">
+        <v>6</v>
+      </c>
+      <c r="B56" s="32" t="s">
+        <v>230</v>
+      </c>
+      <c r="C56" s="12" t="s">
+        <v>231</v>
+      </c>
+      <c r="D56" s="3" t="s">
+        <v>232</v>
+      </c>
+      <c r="E56" s="3"/>
+      <c r="F56" s="12"/>
+      <c r="G56" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="H56" s="12" t="s">
+        <v>233</v>
+      </c>
+      <c r="I56" s="12" t="s">
+        <v>234</v>
+      </c>
+      <c r="J56" s="2" t="s">
+        <v>235</v>
+      </c>
+      <c r="K56" s="6">
+        <v>0.16</v>
+      </c>
+      <c r="L56" s="6">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="M56" s="6">
+        <f>K56*A56</f>
+        <v>0.96</v>
+      </c>
+      <c r="N56" s="6">
+        <f>L56*A56</f>
+        <v>1.0859999999999999</v>
+      </c>
+      <c r="O56" s="4"/>
+      <c r="P56" s="4" t="str">
+        <f>IF(NOT(I56=""),A56&amp;","&amp;I56,"")</f>
+        <v>6,WM9154-ND</v>
+      </c>
+      <c r="Q56" t="str">
+        <f>A56&amp;"x "&amp;C56</f>
+        <v>6x Female pin</v>
+      </c>
+      <c r="R56" t="str">
+        <f>IF(NOT(J56=""),J56&amp;"|"&amp;A56,"")</f>
+        <v>538-39-00-0078|6</v>
+      </c>
+      <c r="S56" t="str">
+        <f>H56&amp;" "&amp;A56</f>
         <v>39-00-0078 6</v>
       </c>
     </row>
-    <row r="56" spans="1:19" ht="24" customHeight="1" thickBot="1">
-      <c r="A56" s="15"/>
-      <c r="B56" s="4"/>
-      <c r="C56" s="3"/>
-      <c r="D56" s="3"/>
-      <c r="E56" s="3"/>
-      <c r="F56" s="20"/>
-      <c r="G56" s="4"/>
-      <c r="H56" s="34" t="s">
+    <row r="57" spans="1:19" ht="24" customHeight="1" thickBot="1">
+      <c r="A57" s="15"/>
+      <c r="B57" s="4"/>
+      <c r="C57" s="3"/>
+      <c r="D57" s="3"/>
+      <c r="E57" s="3"/>
+      <c r="F57" s="20"/>
+      <c r="G57" s="4"/>
+      <c r="H57" s="34" t="s">
         <v>66</v>
       </c>
-      <c r="I56" s="35"/>
-      <c r="J56" s="29"/>
-      <c r="K56" s="1" t="s">
+      <c r="I57" s="35"/>
+      <c r="J57" s="29"/>
+      <c r="K57" s="1" t="s">
         <v>64</v>
       </c>
-      <c r="L56" s="1"/>
-      <c r="M56" s="10">
-        <f>SUM(M3:M51)</f>
+      <c r="L57" s="1"/>
+      <c r="M57" s="10">
+        <f>SUM(M3:M52)</f>
         <v>108.58</v>
       </c>
-      <c r="N56" s="10">
-        <f>SUM(N3:N51)</f>
+      <c r="N57" s="10">
+        <f>SUM(N3:N52)</f>
         <v>125.822</v>
       </c>
-      <c r="O56" s="9" t="s">
+      <c r="O57" s="9" t="s">
         <v>65</v>
-      </c>
-    </row>
-    <row r="60" spans="1:19">
-      <c r="B60" t="s">
-        <v>219</v>
       </c>
     </row>
     <row r="61" spans="1:19">
       <c r="B61" t="s">
-        <v>265</v>
+        <v>219</v>
       </c>
     </row>
     <row r="62" spans="1:19">
       <c r="B62" t="s">
-        <v>242</v>
+        <v>265</v>
       </c>
     </row>
     <row r="63" spans="1:19">
       <c r="B63" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="64" spans="1:19">
+      <c r="B64" t="s">
         <v>264</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
-    <mergeCell ref="H56:I56"/>
+    <mergeCell ref="H57:I57"/>
   </mergeCells>
   <phoneticPr fontId="5" type="noConversion"/>
   <hyperlinks>

</xml_diff>

<commit_message>
Fix on rev 2.0 BOM
</commit_message>
<xml_diff>
--- a/m52 PnP/Rev2.0 documents/BOM-speeduino compatible PCB for m52 rev2.0 sequential.xlsx
+++ b/m52 PnP/Rev2.0 documents/BOM-speeduino compatible PCB for m52 rev2.0 sequential.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pasi\Documents\GitHub\Speeduino-M5x-PCBs\m52 PnP\Rev2.0 documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3732F01C-4E57-4861-BE6A-9843163F1FB4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{339AD80F-DE65-46F0-9A81-AF8D753A9C6F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="14895" yWindow="3825" windowWidth="21600" windowHeight="12735" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Component List" sheetId="1" r:id="rId1"/>
@@ -140,7 +140,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="357" uniqueCount="293">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="363" uniqueCount="300">
   <si>
     <t>Value</t>
   </si>
@@ -1207,6 +1207,27 @@
       </rPr>
       <t>,R71,R73</t>
     </r>
+  </si>
+  <si>
+    <t>Thermal pads</t>
+  </si>
+  <si>
+    <t>Thermal pad</t>
+  </si>
+  <si>
+    <t>Adhesive Thermal Pad for TO-220</t>
+  </si>
+  <si>
+    <t>Aavid</t>
+  </si>
+  <si>
+    <t>53-77-9ACG</t>
+  </si>
+  <si>
+    <t>53-77-9ACG-ND</t>
+  </si>
+  <si>
+    <t>532-53-77-9ACG</t>
   </si>
 </sst>
 </file>
@@ -1979,8 +2000,8 @@
   </sheetPr>
   <dimension ref="A1:S63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
-      <selection activeCell="B32" sqref="B32"/>
+    <sheetView tabSelected="1" topLeftCell="A31" zoomScale="113" zoomScaleNormal="113" workbookViewId="0">
+      <selection activeCell="A50" sqref="A50:XFD50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -4382,7 +4403,7 @@
       </c>
       <c r="O43" s="4"/>
       <c r="P43" s="4" t="str">
-        <f t="shared" ref="P43:P49" si="17">IF(NOT(I43=""),A43&amp;","&amp;I43,"")</f>
+        <f t="shared" ref="P43:P50" si="17">IF(NOT(I43=""),A43&amp;","&amp;I43,"")</f>
         <v>1,MPXH6115A6U-ND</v>
       </c>
       <c r="Q43" t="str">
@@ -4390,7 +4411,7 @@
         <v>1x Baro sensor</v>
       </c>
       <c r="R43" t="str">
-        <f t="shared" ref="R43:R49" si="18">IF(NOT(J43=""),J43&amp;"|"&amp;A43,"")</f>
+        <f t="shared" ref="R43:R50" si="18">IF(NOT(J43=""),J43&amp;"|"&amp;A43,"")</f>
         <v>841-MPXH6115A6U|1</v>
       </c>
       <c r="S43" t="str">
@@ -4698,31 +4719,63 @@
         <v/>
       </c>
     </row>
-    <row r="50" spans="1:19" ht="16.5" thickBot="1">
-      <c r="A50" s="15"/>
-      <c r="B50" s="4" t="s">
-        <v>291</v>
-      </c>
-      <c r="C50" s="3"/>
-      <c r="D50" s="3"/>
+    <row r="50" spans="1:19" ht="16.5" customHeight="1" thickBot="1">
+      <c r="A50" s="17">
+        <v>13</v>
+      </c>
+      <c r="B50" s="11" t="s">
+        <v>293</v>
+      </c>
+      <c r="C50" s="12" t="s">
+        <v>294</v>
+      </c>
+      <c r="D50" s="3" t="s">
+        <v>295</v>
+      </c>
       <c r="E50" s="3"/>
-      <c r="F50" s="3"/>
-      <c r="G50" s="4"/>
-      <c r="H50" s="8"/>
-      <c r="I50" s="3"/>
-      <c r="J50" s="3"/>
-      <c r="K50" s="1"/>
-      <c r="L50" s="1"/>
-      <c r="M50" s="9"/>
-      <c r="N50" s="6"/>
-      <c r="O50" s="9"/>
+      <c r="F50" s="12"/>
+      <c r="G50" s="12" t="s">
+        <v>296</v>
+      </c>
+      <c r="H50" s="12" t="s">
+        <v>297</v>
+      </c>
+      <c r="I50" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>299</v>
+      </c>
+      <c r="K50" s="6">
+        <v>0.55000000000000004</v>
+      </c>
+      <c r="L50" s="6">
+        <v>0.67300000000000004</v>
+      </c>
+      <c r="M50" s="6">
+        <f>K50*A50</f>
+        <v>7.15</v>
+      </c>
+      <c r="N50" s="6">
+        <f>L50*A50</f>
+        <v>8.7490000000000006</v>
+      </c>
+      <c r="O50" s="4"/>
       <c r="P50" s="4" t="str">
-        <f t="shared" ref="P50" si="19">IF(NOT(I50=""),A50&amp;","&amp;I50,"")</f>
-        <v/>
+        <f t="shared" si="17"/>
+        <v>13,53-77-9ACG-ND</v>
+      </c>
+      <c r="Q50" t="str">
+        <f>A50&amp;"x "&amp;C50</f>
+        <v>13x Thermal pad</v>
       </c>
       <c r="R50" t="str">
-        <f t="shared" ref="R50" si="20">IF(NOT(J50=""),J50&amp;"|"&amp;A50,"")</f>
-        <v/>
+        <f t="shared" si="18"/>
+        <v>532-53-77-9ACG|13</v>
+      </c>
+      <c r="S50" t="str">
+        <f>H50&amp;" "&amp;A50</f>
+        <v>53-77-9ACG 13</v>
       </c>
     </row>
     <row r="51" spans="1:19" ht="16.5" thickBot="1">
@@ -5018,11 +5071,11 @@
       <c r="L57" s="1"/>
       <c r="M57" s="10">
         <f>SUM(M3:M52)</f>
-        <v>108.64</v>
+        <v>115.79</v>
       </c>
       <c r="N57" s="10">
         <f>SUM(N3:N52)</f>
-        <v>125.932</v>
+        <v>134.68100000000001</v>
       </c>
       <c r="O57" s="9" t="s">
         <v>65</v>

</xml_diff>